<commit_message>
Update footer and added scrollToTop
</commit_message>
<xml_diff>
--- a/server/customer_data.xlsx
+++ b/server/customer_data.xlsx
@@ -34,13 +34,13 @@
     <t>aliusman@gmail.com</t>
   </si>
   <si>
-    <t>javascript</t>
+    <t>html/css</t>
   </si>
   <si>
     <t>+923331231234</t>
   </si>
   <si>
-    <t>Hello World</t>
+    <t>World</t>
   </si>
 </sst>
 </file>

</xml_diff>